<commit_message>
Add list of mac addresses of demo boards
</commit_message>
<xml_diff>
--- a/boards/boards.xlsx
+++ b/boards/boards.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>SN</t>
   </si>
@@ -96,6 +96,60 @@
   </si>
   <si>
     <t>18:fe:34:d7:68:b8</t>
+  </si>
+  <si>
+    <t>0x00d767c7</t>
+  </si>
+  <si>
+    <t>18:fe:34:d7:67:c7</t>
+  </si>
+  <si>
+    <t>0x001487d5</t>
+  </si>
+  <si>
+    <t>5c:cf:7f:14:87:d5</t>
+  </si>
+  <si>
+    <t>0x000a7895</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5c:cf:7f:0a:78:95</t>
+  </si>
+  <si>
+    <t>0x00d76879</t>
+  </si>
+  <si>
+    <t>18:fe:34:d7:68:79</t>
+  </si>
+  <si>
+    <t>0x00d578d2</t>
+  </si>
+  <si>
+    <t>18:fe:34:d5:78:d2</t>
+  </si>
+  <si>
+    <t>0x00149b1f</t>
+  </si>
+  <si>
+    <t>5c:cf:7f:14:9b:1f</t>
+  </si>
+  <si>
+    <t>0x00d76830</t>
+  </si>
+  <si>
+    <t>18:fe:34:d7:68:30</t>
+  </si>
+  <si>
+    <t>0x00d57af7</t>
+  </si>
+  <si>
+    <t>18:fe:34:d5:7a:f7</t>
+  </si>
+  <si>
+    <t>0x00d57b86</t>
+  </si>
+  <si>
+    <t>18:fe:34:d5:7b:86</t>
   </si>
 </sst>
 </file>
@@ -520,7 +574,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,6 +606,18 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -574,22 +640,52 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -612,17 +708,35 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -636,30 +750,60 @@
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -667,6 +811,9 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>

</xml_diff>

<commit_message>
Add missing boards (15, 9)
</commit_message>
<xml_diff>
--- a/boards/boards.xlsx
+++ b/boards/boards.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SH\MacGyver\projekty\esp8266-board\boards\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="10770"/>
   </bookViews>
   <sheets>
     <sheet name="Boards" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +24,7 @@
     <author>Adam Hořčica</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>SN</t>
   </si>
@@ -150,13 +145,25 @@
   </si>
   <si>
     <t>18:fe:34:d5:7b:86</t>
+  </si>
+  <si>
+    <t>0x000a7262</t>
+  </si>
+  <si>
+    <t>5C:CF:7F:A:72:62</t>
+  </si>
+  <si>
+    <t>0x00d76690</t>
+  </si>
+  <si>
+    <t>18:FE:34:D7:66:90</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,7 +265,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -316,7 +323,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kancelář">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -368,7 +375,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -562,22 +569,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
@@ -585,7 +592,7 @@
     <col min="5" max="5" width="23.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="20.25" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -602,7 +609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -619,7 +626,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -636,7 +643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -653,7 +660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -670,7 +677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -687,7 +694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -704,7 +711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -721,7 +728,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -738,15 +745,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -763,7 +779,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -780,7 +796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -797,7 +813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -808,7 +824,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -819,35 +835,44 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:5">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>

</xml_diff>